<commit_message>
Added WinForms Desktop client for LAB_04 and LAB_05
</commit_message>
<xml_diff>
--- a/LAB_04/число_вхождений.xlsx
+++ b/LAB_04/число_вхождений.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="23700" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Шифр Порты" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
   <si>
     <t>А</t>
   </si>
@@ -134,6 +134,111 @@
   </si>
   <si>
     <t>У</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>ą</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>ć</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>ę</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i </t>
+  </si>
+  <si>
+    <t xml:space="preserve">j </t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>ł</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>ń</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ó </t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>ś</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w  </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>ź</t>
+  </si>
+  <si>
+    <t>ż</t>
   </si>
 </sst>
 </file>
@@ -184,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,6 +298,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -312,215 +421,227 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Шифр Порты'!$A$5:$AG$5</c:f>
+              <c:f>'Шифр Порты'!$A$5:$AI$5</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>А</c:v>
+                  <c:v>a</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Б</c:v>
+                  <c:v>ą</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>В</c:v>
+                  <c:v>b</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Г</c:v>
+                  <c:v>c</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Д</c:v>
+                  <c:v>ć</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Е</c:v>
+                  <c:v>d</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Ё</c:v>
+                  <c:v>e</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Ж</c:v>
+                  <c:v>ę</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>З</c:v>
+                  <c:v>f</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>И</c:v>
+                  <c:v>g</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Й</c:v>
+                  <c:v>h</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>К </c:v>
+                  <c:v>i </c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Л </c:v>
+                  <c:v>j </c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>М</c:v>
+                  <c:v>k</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Н</c:v>
+                  <c:v>l</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>О</c:v>
+                  <c:v>ł</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>П</c:v>
+                  <c:v>m</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Р</c:v>
+                  <c:v>n</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>С</c:v>
+                  <c:v>ń</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Т</c:v>
+                  <c:v>o</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>У </c:v>
+                  <c:v>ó </c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Ф</c:v>
+                  <c:v>p</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Х</c:v>
+                  <c:v>q</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Ц</c:v>
+                  <c:v>r</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Ч</c:v>
+                  <c:v>s</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Ш</c:v>
+                  <c:v>ś</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Щ</c:v>
+                  <c:v>t</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Ъ</c:v>
+                  <c:v>u</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Ы </c:v>
+                  <c:v>v </c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Ь  </c:v>
+                  <c:v>w  </c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Э</c:v>
+                  <c:v>x</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Ю</c:v>
+                  <c:v>y</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Я</c:v>
+                  <c:v>z</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>ź</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>ż</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Шифр Порты'!$A$6:$AG$6</c:f>
+              <c:f>'Шифр Порты'!$A$6:$AI$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>79</c:v>
+                  <c:v>8.3376270000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>1.16632087E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>1.7930006599999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>4.1423536800000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>7.5201583100000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>3.1904965600000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13</c:v>
+                  <c:v>8.1106300000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>1.54163241E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>1.83129776E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52</c:v>
+                  <c:v>1.53327668E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>1.45320091E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51</c:v>
+                  <c:v>8.2136840000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34</c:v>
+                  <c:v>2.5380533199999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21</c:v>
+                  <c:v>2.9593214400000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52</c:v>
+                  <c:v>2.364672E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>95</c:v>
+                  <c:v>1.7811633600000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19</c:v>
+                  <c:v>3.8109097600000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26</c:v>
+                  <c:v>4.8470206600000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>52</c:v>
+                  <c:v>1.64329389E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>56</c:v>
+                  <c:v>7.3502585300000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24</c:v>
+                  <c:v>1.0590889500000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>2.5554612300000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.00E+00">
+                  <c:v>1.3926219300000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.2203407700000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.147228E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0187028900000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.0358181999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.9204255199999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="29">
+                  <c:v>4.017714E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>3.6584176099999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>20</c:v>
+                  <c:v>5.8239449999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.46225293E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.162143E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1122,7 +1243,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1147,103 +1267,103 @@
               <c:strCache>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>А</c:v>
+                  <c:v>a</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Б</c:v>
+                  <c:v>ą</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>В</c:v>
+                  <c:v>b</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Г</c:v>
+                  <c:v>c</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Д</c:v>
+                  <c:v>ć</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Е</c:v>
+                  <c:v>d</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Ё</c:v>
+                  <c:v>e</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Ж</c:v>
+                  <c:v>ę</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>З</c:v>
+                  <c:v>f</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>И</c:v>
+                  <c:v>g</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Й</c:v>
+                  <c:v>h</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>К </c:v>
+                  <c:v>i </c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Л </c:v>
+                  <c:v>j </c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>М</c:v>
+                  <c:v>k</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Н</c:v>
+                  <c:v>l</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>О</c:v>
+                  <c:v>ł</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>П</c:v>
+                  <c:v>m</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Р</c:v>
+                  <c:v>n</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>С</c:v>
+                  <c:v>ń</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Т</c:v>
+                  <c:v>o</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>У </c:v>
+                  <c:v>ó </c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Ф</c:v>
+                  <c:v>p</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Х</c:v>
+                  <c:v>q</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Ц</c:v>
+                  <c:v>r</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Ч</c:v>
+                  <c:v>s</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Ш</c:v>
+                  <c:v>ś</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Щ</c:v>
+                  <c:v>t</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Ъ</c:v>
+                  <c:v>u</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Ы </c:v>
+                  <c:v>v </c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Ь  </c:v>
+                  <c:v>w  </c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Э</c:v>
+                  <c:v>x</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Ю</c:v>
+                  <c:v>y</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Я</c:v>
+                  <c:v>z</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1255,103 +1375,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>79</c:v>
+                  <c:v>8.3376270000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>1.16632087E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>1.7930006599999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>4.1423536800000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>7.5201583100000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51</c:v>
+                  <c:v>3.1904965600000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13</c:v>
+                  <c:v>8.1106300000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>1.54163241E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>1.83129776E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52</c:v>
+                  <c:v>1.53327668E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>1.45320091E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51</c:v>
+                  <c:v>8.2136840000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34</c:v>
+                  <c:v>2.5380533199999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21</c:v>
+                  <c:v>2.9593214400000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52</c:v>
+                  <c:v>2.364672E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>95</c:v>
+                  <c:v>1.7811633600000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19</c:v>
+                  <c:v>3.8109097600000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26</c:v>
+                  <c:v>4.8470206600000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>52</c:v>
+                  <c:v>1.64329389E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>56</c:v>
+                  <c:v>7.3502585300000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24</c:v>
+                  <c:v>1.0590889500000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>2.5554612300000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.00E+00">
+                  <c:v>1.3926219300000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.2203407700000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.147228E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0187028900000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.0358181999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.9204255199999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="29">
+                  <c:v>4.017714E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>3.6584176099999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>20</c:v>
+                  <c:v>5.8239449999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1565,7 +1685,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4645,18 +4764,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AG33"/>
+  <dimension ref="A3:AI33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V38" sqref="V38"/>
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="33" width="5.77734375" customWidth="1"/>
+    <col min="1" max="33" width="5.7109375" customWidth="1"/>
+    <col min="34" max="34" width="5" customWidth="1"/>
+    <col min="35" max="35" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
@@ -4669,209 +4790,221 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>8.3376270000000002E-2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.16632087E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.7930006599999999E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4.1423536800000001E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>7.5201583100000004E-3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3.1904965600000001E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>8.1106300000000006E-2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.54163241E-2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1.83129776E-3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.53327668E-2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1.45320091E-2</v>
+      </c>
+      <c r="L6" s="1">
+        <v>8.2136840000000003E-2</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2.5380533199999999E-2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>2.9593214400000002E-2</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2.364672E-2</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1.7811633600000001E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>3.8109097600000003E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <v>4.8470206600000003E-2</v>
+      </c>
+      <c r="S6" s="1">
+        <v>1.64329389E-3</v>
+      </c>
+      <c r="T6" s="1">
+        <v>7.3502585300000006E-2</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1.0590889500000001E-2</v>
+      </c>
+      <c r="V6" s="1">
+        <v>2.5554612300000001E-2</v>
+      </c>
+      <c r="W6" s="5">
+        <v>1.3926219300000001E-5</v>
+      </c>
+      <c r="X6" s="1">
+        <v>4.2203407700000001E-2</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>4.147228E-2</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1.0187028900000001E-2</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>4.0358181999999999E-2</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1.9204255199999999E-2</v>
+      </c>
+      <c r="AC6" s="1">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG5" s="1" t="s">
-        <v>26</v>
+      <c r="AD6" s="1">
+        <v>4.017714E-2</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>3.6584176099999997E-2</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>5.8239449999999998E-2</v>
+      </c>
+      <c r="AH6" s="4">
+        <v>1.46225293E-3</v>
+      </c>
+      <c r="AI6" s="4">
+        <v>1.162143E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>79</v>
-      </c>
-      <c r="B6" s="1">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1">
-        <v>51</v>
-      </c>
-      <c r="G6" s="1">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1">
-        <v>10</v>
-      </c>
-      <c r="I6" s="1">
-        <v>14</v>
-      </c>
-      <c r="J6" s="1">
-        <v>52</v>
-      </c>
-      <c r="K6" s="1">
-        <v>10</v>
-      </c>
-      <c r="L6" s="1">
-        <v>51</v>
-      </c>
-      <c r="M6" s="1">
-        <v>34</v>
-      </c>
-      <c r="N6" s="1">
-        <v>21</v>
-      </c>
-      <c r="O6" s="1">
-        <v>52</v>
-      </c>
-      <c r="P6" s="1">
-        <v>95</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>19</v>
-      </c>
-      <c r="R6" s="1">
-        <v>26</v>
-      </c>
-      <c r="S6" s="1">
-        <v>52</v>
-      </c>
-      <c r="T6" s="1">
-        <v>56</v>
-      </c>
-      <c r="U6" s="1">
-        <v>24</v>
-      </c>
-      <c r="V6" s="1">
-        <v>0</v>
-      </c>
-      <c r="W6" s="1">
-        <v>3</v>
-      </c>
-      <c r="X6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>17</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>6</v>
-      </c>
-      <c r="AA6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>12</v>
-      </c>
-      <c r="AD6" s="1">
-        <v>9</v>
-      </c>
-      <c r="AE6" s="1">
-        <v>3</v>
-      </c>
-      <c r="AF6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -4899,7 +5032,7 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -4927,7 +5060,7 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E31" s="3" t="s">
         <v>34</v>
       </c>
@@ -4942,7 +5075,7 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -4974,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>169</v>
       </c>
@@ -5024,9 +5157,9 @@
       <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F1" s="3" t="s">
         <v>33</v>
       </c>
@@ -5039,7 +5172,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5140,7 +5273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>79</v>
       </c>
@@ -5241,7 +5374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -5269,7 +5402,7 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -5297,7 +5430,7 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="F29" s="3" t="s">
         <v>34</v>
       </c>
@@ -5312,7 +5445,7 @@
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -5413,7 +5546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Change GetKey method in MultiPermCrypt class
</commit_message>
<xml_diff>
--- a/LAB_04/число_вхождений.xlsx
+++ b/LAB_04/число_вхождений.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23700" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="23700" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Шифр Порты" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
   <si>
     <t>А</t>
   </si>
@@ -297,11 +297,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -337,27 +337,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="7.9897493128319591E-2"/>
-          <c:y val="5.6798012069577568E-2"/>
-          <c:w val="0.91354082708165418"/>
-          <c:h val="0.87860039859234851"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -365,60 +355,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="dk1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="ru-RU"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'Шифр Порты'!$A$5:$AI$5</c:f>
@@ -648,26 +584,25 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9E4D-4F77-A055-7D570BCE8619}"/>
+              <c16:uniqueId val="{00000000-202C-4B4E-90B1-B23ECF67238A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
-        <c:axId val="1292778064"/>
-        <c:axId val="1292783056"/>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="396966984"/>
+        <c:axId val="396965016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1292778064"/>
+        <c:axId val="396966984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +614,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -697,7 +632,10 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -707,7 +645,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292783056"/>
+        <c:crossAx val="396965016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -715,7 +653,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1292783056"/>
+        <c:axId val="396965016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,7 +691,10 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -763,7 +704,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292778064"/>
+        <c:crossAx val="396966984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -780,38 +721,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="accent4">
-            <a:lumMod val="110000"/>
-            <a:satMod val="105000"/>
-            <a:tint val="67000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="50000">
-          <a:schemeClr val="accent4">
-            <a:lumMod val="105000"/>
-            <a:satMod val="103000"/>
-            <a:tint val="73000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="accent4">
-            <a:lumMod val="105000"/>
-            <a:satMod val="109000"/>
-            <a:tint val="81000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:lin ang="5400000" scaled="0"/>
-    </a:gradFill>
-    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="accent4"/>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:miter lim="800000"/>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -820,14 +740,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr>
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:latin typeface="+mn-lt"/>
-          <a:ea typeface="+mn-ea"/>
-          <a:cs typeface="+mn-cs"/>
-        </a:defRPr>
+        <a:defRPr/>
       </a:pPr>
       <a:endParaRPr lang="ru-RU"/>
     </a:p>
@@ -865,139 +778,245 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:pattFill prst="narHorz">
-              <a:fgClr>
-                <a:schemeClr val="accent1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
-              </a:bgClr>
-            </a:pattFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:innerShdw blurRad="114300">
-                <a:schemeClr val="accent1"/>
-              </a:innerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Шифр Порты'!$A$32:$AI$32</c:f>
+              <c:strCache>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ą</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>c</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ć</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>d</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>e</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ę</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>f</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>g</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>h</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>i </c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>j </c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>l</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>ł</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>m</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>n</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>ń</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>o</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>ó </c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>p</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>q</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>r</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>s</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>ś</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>t</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>u</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>v </c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>w  </c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>x</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>y</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>z</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>ź</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>ż</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Шифр Порты'!$A$32:$J$32</c:f>
+              <c:f>'Шифр Порты'!$A$33:$AI$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.5419530000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1.837813E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>1.53359929E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>1.453543E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>8.2123786200000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>2.53813118E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>2.9592966700000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>2.3647919999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>1.7814256300000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3.8106772999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.8465356199999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6498548200000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.3491630000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.059527E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5555346199999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00E+00">
+                  <c:v>2.0884239999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.2200084800000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.1469138099999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.01915086E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.0355309999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9206538799999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00E+00">
+                  <c:v>6.9614129999999997E-6</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.00E+00">
+                  <c:v>4.0174312900000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="0.00E+00">
+                  <c:v>6.9614129999999997E-6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.6582224099999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.8232218000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.4688581E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.16255591E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.3362919999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.1667327999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.79326E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.14204076E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.5252870000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.1904153499999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.1093499999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6B78-43DE-99AE-EBAA80D1C4BC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:pattFill prst="narHorz">
-              <a:fgClr>
-                <a:schemeClr val="accent2"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:innerShdw blurRad="114300">
-                <a:schemeClr val="accent2"/>
-              </a:innerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Шифр Порты'!$A$33:$J$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>152</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>161</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>166</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6B78-43DE-99AE-EBAA80D1C4BC}"/>
+              <c16:uniqueId val="{00000000-F0B4-46F8-814A-40629C7C0829}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1011,26 +1030,27 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="715140624"/>
-        <c:axId val="715138544"/>
+        <c:axId val="514104216"/>
+        <c:axId val="514103560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="715140624"/>
+        <c:axId val="514104216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1057,7 +1077,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="715138544"/>
+        <c:crossAx val="514103560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1065,7 +1085,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="715138544"/>
+        <c:axId val="514103560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1073,13 +1093,14 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -1115,7 +1136,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="715140624"/>
+        <c:crossAx val="514104216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2309,7 +2330,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="340">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2320,7 +2341,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2333,7 +2354,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -2350,7 +2371,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2366,7 +2387,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2410,35 +2431,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2450,31 +2471,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2514,22 +2534,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2576,8 +2597,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -2628,8 +2655,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2667,20 +2694,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2693,17 +2720,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2735,7 +2751,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2744,13 +2760,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2771,19 +2788,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2804,14 +2822,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="299">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2822,7 +2846,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2835,11 +2859,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2852,7 +2876,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2868,7 +2892,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2912,72 +2936,32 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="narHorz">
-        <a:fgClr>
-          <a:schemeClr val="phClr"/>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="phClr">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:innerShdw blurRad="114300">
-          <a:schemeClr val="phClr"/>
-        </a:innerShdw>
-      </a:effectLst>
-    </cs:spPr>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="phClr"/>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="phClr">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -2989,29 +2973,33 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3033,13 +3021,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3049,7 +3039,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3058,25 +3048,135 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -3084,117 +3184,6 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3215,7 +3204,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -3223,7 +3212,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3243,10 +3232,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -3263,11 +3252,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3276,13 +3265,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3303,19 +3293,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3336,8 +3327,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -4373,20 +4370,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4403,20 +4400,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Диаграмма 3"/>
+        <xdr:cNvPr id="6" name="Диаграмма 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4764,10 +4761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AI33"/>
+  <dimension ref="A5:AI36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="S62" sqref="S62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4777,19 +4774,6 @@
     <col min="35" max="35" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="F3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-    </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>38</v>
@@ -4964,7 +4948,7 @@
       <c r="V6" s="1">
         <v>2.5554612300000001E-2</v>
       </c>
-      <c r="W6" s="5">
+      <c r="W6" s="4">
         <v>1.3926219300000001E-5</v>
       </c>
       <c r="X6" s="1">
@@ -4997,29 +4981,20 @@
       <c r="AG6" s="1">
         <v>5.8239449999999998E-2</v>
       </c>
-      <c r="AH6" s="4">
+      <c r="AH6" s="3">
         <v>1.46225293E-3</v>
       </c>
-      <c r="AI6" s="4">
+      <c r="AI6" s="3">
         <v>1.162143E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -5032,7 +5007,7 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -5060,89 +5035,250 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E31" s="3" t="s">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI32" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>1.5419530000000001E-2</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.837813E-3</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1.53359929E-2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1.453543E-2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>8.2123786200000007E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2.53813118E-2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2.9592966700000001E-2</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2.3647919999999999E-2</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1.7814256300000001E-2</v>
+      </c>
+      <c r="J33" s="1">
+        <v>3.8106772999999997E-2</v>
+      </c>
+      <c r="K33" s="1">
+        <v>4.8465356199999997E-2</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1.6498548200000001E-3</v>
+      </c>
+      <c r="M33" s="1">
+        <v>7.3491630000000002E-2</v>
+      </c>
+      <c r="N33" s="1">
+        <v>1.059527E-2</v>
+      </c>
+      <c r="O33" s="1">
+        <v>2.5555346199999999E-2</v>
+      </c>
+      <c r="P33" s="4">
+        <v>2.0884239999999998E-5</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>4.2200084800000003E-2</v>
+      </c>
+      <c r="R33" s="1">
+        <v>4.1469138099999997E-2</v>
+      </c>
+      <c r="S33" s="1">
+        <v>1.01915086E-2</v>
+      </c>
+      <c r="T33" s="1">
+        <v>4.0355309999999998E-2</v>
+      </c>
+      <c r="U33" s="1">
+        <v>1.9206538799999999E-2</v>
+      </c>
+      <c r="V33" s="4">
+        <v>6.9614129999999997E-6</v>
+      </c>
+      <c r="W33" s="4">
+        <v>4.0174312900000002E-2</v>
+      </c>
+      <c r="X33" s="4">
+        <v>6.9614129999999997E-6</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>3.6582224099999998E-2</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>5.8232218000000002E-2</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>1.4688581E-3</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>1.16255591E-2</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>8.3362919999999993E-2</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>1.1667327999999999E-2</v>
+      </c>
+      <c r="AE33" s="1">
+        <v>1.79326E-2</v>
+      </c>
+      <c r="AF33" s="1">
+        <v>4.14204076E-2</v>
+      </c>
+      <c r="AG33" s="1">
+        <v>7.5252870000000003E-3</v>
+      </c>
+      <c r="AH33" s="3">
+        <v>3.1904153499999997E-2</v>
+      </c>
+      <c r="AI33" s="3">
+        <v>8.1093499999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="G36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="T36" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>1</v>
-      </c>
-      <c r="B32" s="1">
-        <v>2</v>
-      </c>
-      <c r="C32" s="1">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1">
-        <v>4</v>
-      </c>
-      <c r="E32" s="1">
-        <v>5</v>
-      </c>
-      <c r="F32" s="1">
-        <v>6</v>
-      </c>
-      <c r="G32" s="1">
-        <v>7</v>
-      </c>
-      <c r="H32" s="1">
-        <v>8</v>
-      </c>
-      <c r="I32" s="1">
-        <v>9</v>
-      </c>
-      <c r="J32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>169</v>
-      </c>
-      <c r="B33" s="1">
-        <v>94</v>
-      </c>
-      <c r="C33" s="1">
-        <v>152</v>
-      </c>
-      <c r="D33" s="1">
-        <v>148</v>
-      </c>
-      <c r="E33" s="1">
-        <v>116</v>
-      </c>
-      <c r="F33" s="1">
-        <v>161</v>
-      </c>
-      <c r="G33" s="1">
-        <v>103</v>
-      </c>
-      <c r="H33" s="1">
-        <v>75</v>
-      </c>
-      <c r="I33" s="1">
-        <v>63</v>
-      </c>
-      <c r="J33" s="1">
-        <v>166</v>
-      </c>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="5"/>
+      <c r="AC36" s="5"/>
+      <c r="AD36" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F3:N3"/>
-    <mergeCell ref="E31:O31"/>
+    <mergeCell ref="G36:O36"/>
+    <mergeCell ref="T36:AD36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5160,17 +5296,17 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -5431,19 +5567,19 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">

</xml_diff>